<commit_message>
Terminada reorganización del repositorio. Empiezo a estudiar correlaciones
</commit_message>
<xml_diff>
--- a/Aplicación/Datos/Datos NOAA Buoy Data/BAY OF CAMPECHE/Correlaciones.xlsx
+++ b/Aplicación/Datos/Datos NOAA Buoy Data/BAY OF CAMPECHE/Correlaciones.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\_____Publicaciones y Tesis\Aerogeneradores\Modelo Datos\Datos NOAA Buoy Data\BAY OF CAMPECHE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\_____Publicaciones y Tesis\Aerogeneradores\Modelo Datos\Aplicación\Datos\Datos NOAA Buoy Data\BAY OF CAMPECHE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5C81E14D-3ED2-4C52-846A-36A6ADA9D043}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C32EFA47-E504-4543-BEF3-992557690208}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8964" xr2:uid="{246B54E7-5A5F-45B8-A959-D9568FA482E6}"/>
   </bookViews>

</xml_diff>